<commit_message>
fix alasan jika ditolak
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_gedung - Copy.xlsx
+++ b/public/templates/template_aset_gedung - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31FF8EE-ACA2-4F00-9981-C886FC05CBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDFC0C2-2A41-468D-AE23-982F9BEA4322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{704EB8C1-9152-478B-B06B-65132D1E22AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>id_status_aset</t>
   </si>
@@ -78,9 +78,6 @@
     <t>02.02.0001</t>
   </si>
   <si>
-    <t>Kantor PUSDIKLAT Kendalisada</t>
-  </si>
-  <si>
     <t>23/11/2023</t>
   </si>
   <si>
@@ -115,6 +112,15 @@
   </si>
   <si>
     <t>23/11/2025</t>
+  </si>
+  <si>
+    <t>Kantor PUSDIKLAT Kendalisada 1</t>
+  </si>
+  <si>
+    <t>Kantor PUSDIKLAT Kendalisada 2</t>
+  </si>
+  <si>
+    <t>Kantor PUSDIKLAT Kendalisada 3</t>
   </si>
 </sst>
 </file>
@@ -482,14 +488,14 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
@@ -560,43 +566,43 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
       </c>
       <c r="H2">
         <v>106</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2">
         <v>1963</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2">
         <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -604,46 +610,46 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
       </c>
       <c r="H3">
         <v>107</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3">
         <v>1964</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3">
         <v>176</v>
       </c>
       <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>24</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -651,46 +657,46 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
       <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
       </c>
       <c r="H4">
         <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4">
         <v>1965</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4">
         <v>177</v>
       </c>
       <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>24</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>